<commit_message>
Überarbeitung Basisworkflow. Neue Argumente für die jeweiligen Portalsuchen definiert.
</commit_message>
<xml_diff>
--- a/CF_Public_Tender_Research/Data/Config.xlsx
+++ b/CF_Public_Tender_Research/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrose\Documents\UiPath\CF_Public_Tender_Research\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrose\Documents\Github\CF Portal Search\CF_Public_Tender_Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1576,7 +1576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1626,7 +1628,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -2788,7 +2790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>